<commit_message>
Update backlogs to 30 user stories per sprint with proper team distribution
Co-authored-by: HarshChoudhary10 <144003686+HarshChoudhary10@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/PB.xlsx
+++ b/PB.xlsx
@@ -444,7 +444,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:M93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -566,12 +566,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Set up the project repository and environment</t>
+          <t>initialize the GitHub repository</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>the team can collaborate effectively</t>
+          <t>the team can start collaborating</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -579,7 +579,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Team Lead</t>
+          <t>HC</t>
         </is>
       </c>
       <c r="H4" s="4" t="n">
@@ -612,12 +612,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Create scripts to scrape course content from TDS website</t>
+          <t>set up the local development environment</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>we can build the knowledge base with course materials</t>
+          <t>I can start coding</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -625,20 +625,20 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Developer 1</t>
+          <t>HC</t>
         </is>
       </c>
       <c r="H5" s="4" t="n">
-        <v>45674</v>
+        <v>45672</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Developer A</t>
+          <t>Harsh Choudhary</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>DA</t>
+          <t>HC</t>
         </is>
       </c>
     </row>
@@ -658,12 +658,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Create scripts to scrape Discourse forum posts</t>
+          <t>create a comprehensive README</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>we can include forum discussions in the knowledge base</t>
+          <t>team members understand the project</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -671,20 +671,20 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Developer 2</t>
+          <t>HC</t>
         </is>
       </c>
       <c r="H6" s="4" t="n">
-        <v>45675</v>
+        <v>45673</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Developer B</t>
+          <t>Harsh Choudhary</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>DB</t>
+          <t>HC</t>
         </is>
       </c>
     </row>
@@ -704,33 +704,33 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Implement date range filtering for Discourse posts</t>
+          <t>set up requirements.txt</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>we can scrape posts from specific time periods</t>
+          <t>dependencies are managed properly</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Developer 2</t>
+          <t>HC</t>
         </is>
       </c>
       <c r="H7" s="4" t="n">
-        <v>45676</v>
+        <v>45673</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Developer B</t>
+          <t>Harsh Choudhary</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>DB</t>
+          <t>HC</t>
         </is>
       </c>
     </row>
@@ -750,12 +750,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Test and validate scraped data quality</t>
+          <t>create .gitignore file</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>we ensure accurate data for the knowledge base</t>
+          <t>unnecessary files are not committed</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -763,30 +763,30 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>QA Lead</t>
+          <t>HC</t>
         </is>
       </c>
       <c r="H8" s="4" t="n">
-        <v>45677</v>
+        <v>45673</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Tester C</t>
+          <t>Harsh Choudhary</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>TC</t>
+          <t>HC</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>SB2/US1</t>
+          <t>SB1/US6</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -796,12 +796,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Design the SQLite database schema for the knowledge base</t>
+          <t>research the TDS course website structure</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>we can store course and forum data efficiently</t>
+          <t>I can plan the scraping strategy</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -809,30 +809,30 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Developer 1</t>
+          <t>HC</t>
         </is>
       </c>
       <c r="H9" s="4" t="n">
-        <v>45679</v>
+        <v>45674</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Developer A</t>
+          <t>Harsh Choudhary</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>DA</t>
+          <t>HC</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>SB2/US2</t>
+          <t>SB1/US7</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -842,12 +842,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Implement text chunking functionality</t>
+          <t>create website scraper script</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>we can break down long documents into manageable pieces</t>
+          <t>course content can be downloaded</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -855,30 +855,30 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Developer 1</t>
+          <t>HC</t>
         </is>
       </c>
       <c r="H10" s="4" t="n">
-        <v>45680</v>
+        <v>45675</v>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Developer A</t>
+          <t>Harsh Choudhary</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>DA</t>
+          <t>HC</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>SB2/US3</t>
+          <t>SB1/US8</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -888,12 +888,12 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Integrate SentenceTransformer for local embeddings</t>
+          <t>implement HTML to Markdown conversion</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>we can generate embeddings without external API dependencies</t>
+          <t>content is in usable format</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -901,30 +901,30 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Developer 2</t>
+          <t>HC</t>
         </is>
       </c>
       <c r="H11" s="4" t="n">
-        <v>45681</v>
+        <v>45676</v>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Developer B</t>
+          <t>Harsh Choudhary</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>DB</t>
+          <t>HC</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>SB2/US4</t>
+          <t>SB1/US9</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -934,12 +934,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Create knowledge base creation script</t>
+          <t>add error handling to scraper</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>we can populate the database with chunked and embedded content</t>
+          <t>failures are managed gracefully</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -947,30 +947,30 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Developer 1</t>
+          <t>HC</t>
         </is>
       </c>
       <c r="H12" s="4" t="n">
-        <v>45682</v>
+        <v>45676</v>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Developer A</t>
+          <t>Harsh Choudhary</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>DA</t>
+          <t>HC</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>SB2/US5</t>
+          <t>SB1/US10</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -980,12 +980,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Implement URL update functionality for Discourse links</t>
+          <t>implement rate limiting</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>all forum links work correctly</t>
+          <t>the website is not overloaded</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -993,30 +993,30 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Developer 2</t>
+          <t>HC</t>
         </is>
       </c>
       <c r="H13" s="4" t="n">
-        <v>45683</v>
+        <v>45677</v>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Developer B</t>
+          <t>Harsh Choudhary</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>DB</t>
+          <t>HC</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>SB2/US6</t>
+          <t>SB1/US11</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1026,43 +1026,43 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Test embedding quality and retrieval accuracy</t>
+          <t>create metadata.json file</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>we ensure relevant content is retrieved for queries</t>
+          <t>scraped data is tracked</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>QA Lead</t>
+          <t>HC</t>
         </is>
       </c>
       <c r="H14" s="4" t="n">
-        <v>45684</v>
+        <v>45677</v>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Tester C</t>
+          <t>Harsh Choudhary</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>TC</t>
+          <t>HC</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>SB3/US1</t>
+          <t>SB1/US12</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1072,12 +1072,12 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Create FastAPI application structure</t>
+          <t>research Discourse API</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>we can build the REST API for the Virtual TA</t>
+          <t>forum posts can be scraped</t>
         </is>
       </c>
       <c r="F15" t="n">
@@ -1085,30 +1085,30 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Developer 1</t>
+          <t>HC</t>
         </is>
       </c>
       <c r="H15" s="4" t="n">
-        <v>45686</v>
+        <v>45677</v>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Developer A</t>
+          <t>Harsh Choudhary</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>DA</t>
+          <t>HC</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>SB3/US2</t>
+          <t>SB1/US13</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1118,12 +1118,12 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Implement semantic search with embeddings</t>
+          <t>implement Discourse API authentication</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>users can get relevant answers based on their questions</t>
+          <t>posts can be accessed</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -1131,30 +1131,30 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Developer 1</t>
+          <t>HC</t>
         </is>
       </c>
       <c r="H16" s="4" t="n">
-        <v>45687</v>
+        <v>45678</v>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>Developer A</t>
+          <t>Harsh Choudhary</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>DA</t>
+          <t>HC</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>SB3/US3</t>
+          <t>SB1/US14</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1164,43 +1164,43 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Integrate OCR capability for image processing</t>
+          <t>create discourse_by_date_range.py</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>users can ask questions with screenshots</t>
+          <t>posts can be scraped by date</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Developer 2</t>
+          <t>HC</t>
         </is>
       </c>
       <c r="H17" s="4" t="n">
-        <v>45688</v>
+        <v>45678</v>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Developer B</t>
+          <t>Harsh Choudhary</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>DB</t>
+          <t>HC</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>SB3/US4</t>
+          <t>SB1/US15</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1210,12 +1210,12 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Implement LLM integration for answer generation</t>
+          <t>implement pagination for Discourse API</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>the system provides coherent answers with proper citations</t>
+          <t>all posts are retrieved</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -1223,30 +1223,30 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Developer 1</t>
+          <t>HC</t>
         </is>
       </c>
       <c r="H18" s="4" t="n">
-        <v>45689</v>
+        <v>45679</v>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Developer A</t>
+          <t>Harsh Choudhary</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>DA</t>
+          <t>HC</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>SB3/US5</t>
+          <t>SB1/US16</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1256,43 +1256,43 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Add CORS middleware and security features</t>
+          <t>create discourse_by_post_id.py</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>the API is secure and accessible from web applications</t>
+          <t>specific posts can be scraped</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Developer 2</t>
+          <t>GM</t>
         </is>
       </c>
       <c r="H19" s="4" t="n">
-        <v>45690</v>
+        <v>45679</v>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Developer B</t>
+          <t>Gaurav Malik</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>DB</t>
+          <t>GM</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>SB3/US6</t>
+          <t>SB1/US17</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1302,12 +1302,12 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Implement logging and error handling</t>
+          <t>extract post metadata</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>we can monitor and debug the application effectively</t>
+          <t>context is preserved</t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -1315,122 +1315,122 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Developer 2</t>
+          <t>GM</t>
         </is>
       </c>
       <c r="H20" s="4" t="n">
-        <v>45691</v>
+        <v>45680</v>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Developer B</t>
+          <t>Gaurav Malik</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>DB</t>
+          <t>GM</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>SB3/US7</t>
+          <t>SB1/US18</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>User</t>
+          <t>Developer</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Query the Virtual TA with text questions</t>
+          <t>handle Discourse API rate limits</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>I can get answers from course materials and forums</t>
+          <t>scraping continues smoothly</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Developer 1</t>
+          <t>GM</t>
         </is>
       </c>
       <c r="H21" s="4" t="n">
-        <v>45692</v>
+        <v>45680</v>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>Developer A</t>
+          <t>Gaurav Malik</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>DA</t>
+          <t>GM</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>SB3/US8</t>
+          <t>SB1/US19</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>User</t>
+          <t>Developer</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Include images in my questions</t>
+          <t>create data validation tests</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>I can get help with visual content like diagrams</t>
+          <t>scraped data quality is verified</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Developer 2</t>
+          <t>GM</t>
         </is>
       </c>
       <c r="H22" s="4" t="n">
-        <v>45692</v>
+        <v>45681</v>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>Developer B</t>
+          <t>Gaurav Malik</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>DB</t>
+          <t>GM</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>SB4/US1</t>
+          <t>SB1/US20</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1440,12 +1440,12 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Create Dockerfile for containerization</t>
+          <t>verify course content completeness</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>the application can be deployed easily</t>
+          <t>no pages are missed</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -1453,30 +1453,30 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>DevOps Lead</t>
+          <t>GM</t>
         </is>
       </c>
       <c r="H23" s="4" t="n">
-        <v>45694</v>
+        <v>45681</v>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>DevOps D</t>
+          <t>Gaurav Malik</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>DD</t>
+          <t>GM</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>SB4/US2</t>
+          <t>SB1/US21</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1486,12 +1486,12 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Set up deployment on Render/Cloud platform</t>
+          <t>validate forum post data integrity</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>the Virtual TA is accessible to students</t>
+          <t>all fields are present</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -1499,30 +1499,30 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>DevOps Lead</t>
+          <t>GM</t>
         </is>
       </c>
       <c r="H24" s="4" t="n">
-        <v>45696</v>
+        <v>45682</v>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>DevOps D</t>
+          <t>Gaurav Malik</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>DD</t>
+          <t>GM</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>SB4/US3</t>
+          <t>SB1/US22</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1532,58 +1532,58 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Implement comprehensive API testing</t>
+          <t>create sample data viewer</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>all endpoints work correctly</t>
+          <t>scraped content can be inspected</t>
         </is>
       </c>
       <c r="F25" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>QA Lead</t>
+          <t>GM</t>
         </is>
       </c>
       <c r="H25" s="4" t="n">
-        <v>45697</v>
+        <v>45682</v>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>Tester C</t>
+          <t>Gaurav Malik</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>TC</t>
+          <t>GM</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>SB4/US4</t>
+          <t>SB1/US23</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>User</t>
+          <t>Developer</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Access the Virtual TA through a web interface</t>
+          <t>implement incremental scraping</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>I can easily ask questions without technical knowledge</t>
+          <t>only new content is downloaded</t>
         </is>
       </c>
       <c r="F26" t="n">
@@ -1591,30 +1591,30 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Developer 1</t>
+          <t>DS</t>
         </is>
       </c>
       <c r="H26" s="4" t="n">
-        <v>45698</v>
+        <v>45683</v>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>Developer A</t>
+          <t>Deepanshu Sharma</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>DA</t>
+          <t>DS</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>SB4/US5</t>
+          <t>SB1/US24</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1624,43 +1624,43 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Create comprehensive documentation</t>
+          <t>handle special characters in content</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>users and developers understand how to use and maintain the system</t>
+          <t>text is properly encoded</t>
         </is>
       </c>
       <c r="F27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Tech Writer</t>
+          <t>DS</t>
         </is>
       </c>
       <c r="H27" s="4" t="n">
-        <v>45699</v>
+        <v>45683</v>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>Writer E</t>
+          <t>Deepanshu Sharma</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>WE</t>
+          <t>DS</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>SB4/US6</t>
+          <t>SB1/US25</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1670,12 +1670,12 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Monitor and optimize performance</t>
+          <t>extract code blocks from posts</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>the system responds quickly to user queries</t>
+          <t>they are properly formatted</t>
         </is>
       </c>
       <c r="F28" t="n">
@@ -1683,20 +1683,3010 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>DevOps Lead</t>
+          <t>DS</t>
         </is>
       </c>
       <c r="H28" s="4" t="n">
+        <v>45684</v>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>Deepanshu Sharma</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>1</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>SB1/US26</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>extract links from content</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>references are preserved</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>2</v>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+      <c r="H29" s="4" t="n">
+        <v>45684</v>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>Deepanshu Sharma</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>1</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>SB1/US27</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>implement data cleaning</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>scraped content is ready for processing</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
+        <v>1</v>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+      <c r="H30" s="4" t="n">
+        <v>45685</v>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>Deepanshu Sharma</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>1</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>SB1/US28</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>create scraping configuration file</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>settings are centralized</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>2</v>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+      <c r="H31" s="4" t="n">
+        <v>45685</v>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>Deepanshu Sharma</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>1</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>SB1/US29</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>add progress tracking</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>scraping status is visible</t>
+        </is>
+      </c>
+      <c r="F32" t="n">
+        <v>2</v>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+      <c r="H32" s="4" t="n">
+        <v>45686</v>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>Deepanshu Sharma</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>1</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>SB1/US30</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>create backup mechanism</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>scraped data is not lost</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>1</v>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+      <c r="H33" s="4" t="n">
+        <v>45687</v>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>Deepanshu Sharma</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>2</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>SB2/US1</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>design the database schema</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>data can be stored efficiently</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
+        <v>1</v>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H34" s="4" t="n">
+        <v>45688</v>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>2</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>SB2/US2</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>create SQLite database file</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>data can be persisted</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
+        <v>1</v>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H35" s="4" t="n">
+        <v>45689</v>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>2</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>SB2/US3</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>implement text chunking</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>long documents are split properly</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
+        <v>1</v>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H36" s="4" t="n">
+        <v>45690</v>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>2</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>SB2/US4</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>handle special cases in chunking</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>text boundaries are respected</t>
+        </is>
+      </c>
+      <c r="F37" t="n">
+        <v>1</v>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H37" s="4" t="n">
+        <v>45691</v>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>2</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>SB2/US5</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>research embedding models</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>the best one is selected</t>
+        </is>
+      </c>
+      <c r="F38" t="n">
+        <v>1</v>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H38" s="4" t="n">
+        <v>45692</v>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>2</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>SB2/US6</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>implement local embedding generation</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>no external API is needed</t>
+        </is>
+      </c>
+      <c r="F39" t="n">
+        <v>1</v>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H39" s="4" t="n">
+        <v>45693</v>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>2</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>SB2/US7</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>add GPU support</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>embedding generation is faster</t>
+        </is>
+      </c>
+      <c r="F40" t="n">
+        <v>2</v>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H40" s="4" t="n">
+        <v>45694</v>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>2</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>SB2/US8</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>implement batch embedding</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>processing is efficient</t>
+        </is>
+      </c>
+      <c r="F41" t="n">
+        <v>1</v>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H41" s="4" t="n">
+        <v>45695</v>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>2</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>SB2/US9</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>create base_creation_test.py</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>knowledge base can be built</t>
+        </is>
+      </c>
+      <c r="F42" t="n">
+        <v>1</v>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H42" s="4" t="n">
+        <v>45696</v>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>2</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>SB2/US10</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>process course content</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>it is added to knowledge base</t>
+        </is>
+      </c>
+      <c r="F43" t="n">
+        <v>1</v>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H43" s="4" t="n">
+        <v>45697</v>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>2</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>SB2/US11</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>process forum posts</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>they are added to knowledge base</t>
+        </is>
+      </c>
+      <c r="F44" t="n">
+        <v>1</v>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H44" s="4" t="n">
+        <v>45698</v>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>2</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>SB2/US12</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>store embeddings in database</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>they can be queried later</t>
+        </is>
+      </c>
+      <c r="F45" t="n">
+        <v>1</v>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H45" s="4" t="n">
+        <v>45699</v>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>2</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>SB2/US13</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>implement progress tracking</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>knowledge base creation can be monitored</t>
+        </is>
+      </c>
+      <c r="F46" t="n">
+        <v>2</v>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H46" s="4" t="n">
         <v>45700</v>
       </c>
-      <c r="K28" t="inlineStr">
-        <is>
-          <t>DevOps D</t>
-        </is>
-      </c>
-      <c r="L28" t="inlineStr">
-        <is>
-          <t>DD</t>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>2</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>SB2/US14</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>handle duplicate content</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>knowledge base is clean</t>
+        </is>
+      </c>
+      <c r="F47" t="n">
+        <v>2</v>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H47" s="4" t="n">
+        <v>45701</v>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>2</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>SB2/US15</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>implement updatelinks.py</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Discourse URLs are corrected</t>
+        </is>
+      </c>
+      <c r="F48" t="n">
+        <v>1</v>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H48" s="4" t="n">
+        <v>45702</v>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>2</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>SB2/US16</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>test URL updates</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>all links are working</t>
+        </is>
+      </c>
+      <c r="F49" t="n">
+        <v>1</v>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>GM</t>
+        </is>
+      </c>
+      <c r="H49" s="4" t="n">
+        <v>45703</v>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>Gaurav Malik</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>GM</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>2</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>SB2/US17</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>create embedding quality tests</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>retrieval accuracy is verified</t>
+        </is>
+      </c>
+      <c r="F50" t="n">
+        <v>1</v>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>GM</t>
+        </is>
+      </c>
+      <c r="H50" s="4" t="n">
+        <v>45704</v>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>Gaurav Malik</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>GM</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>2</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>SB2/US18</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>implement cosine similarity function</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>embeddings can be compared</t>
+        </is>
+      </c>
+      <c r="F51" t="n">
+        <v>1</v>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>GM</t>
+        </is>
+      </c>
+      <c r="H51" s="4" t="n">
+        <v>45705</v>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>Gaurav Malik</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>GM</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>2</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>SB2/US19</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>test retrieval with sample queries</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>knowledge base works correctly</t>
+        </is>
+      </c>
+      <c r="F52" t="n">
+        <v>1</v>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>GM</t>
+        </is>
+      </c>
+      <c r="H52" s="4" t="n">
+        <v>45706</v>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>Gaurav Malik</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>GM</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>2</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>SB2/US20</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>implement similarity threshold</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>irrelevant results are filtered</t>
+        </is>
+      </c>
+      <c r="F53" t="n">
+        <v>1</v>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>GM</t>
+        </is>
+      </c>
+      <c r="H53" s="4" t="n">
+        <v>45707</v>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>Gaurav Malik</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>GM</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>2</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>SB2/US21</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>add metadata extraction</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>source info is preserved</t>
+        </is>
+      </c>
+      <c r="F54" t="n">
+        <v>2</v>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>GM</t>
+        </is>
+      </c>
+      <c r="H54" s="4" t="n">
+        <v>45708</v>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>Gaurav Malik</t>
+        </is>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>GM</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>2</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>SB2/US22</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>implement database indexing</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>queries are fast</t>
+        </is>
+      </c>
+      <c r="F55" t="n">
+        <v>1</v>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>GM</t>
+        </is>
+      </c>
+      <c r="H55" s="4" t="n">
+        <v>45709</v>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>Gaurav Malik</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>GM</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>2</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>SB2/US23</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>add database backup functionality</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>data is safe</t>
+        </is>
+      </c>
+      <c r="F56" t="n">
+        <v>2</v>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+      <c r="H56" s="4" t="n">
+        <v>45710</v>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>Deepanshu Sharma</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>2</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>SB2/US24</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>create database statistics script</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>content can be analyzed</t>
+        </is>
+      </c>
+      <c r="F57" t="n">
+        <v>2</v>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+      <c r="H57" s="4" t="n">
+        <v>45711</v>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>Deepanshu Sharma</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>2</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>SB2/US25</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>implement error handling</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>processing continues on failures</t>
+        </is>
+      </c>
+      <c r="F58" t="n">
+        <v>1</v>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+      <c r="H58" s="4" t="n">
+        <v>45712</v>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>Deepanshu Sharma</t>
+        </is>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>2</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>SB2/US26</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>optimize memory usage</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>large datasets can be processed</t>
+        </is>
+      </c>
+      <c r="F59" t="n">
+        <v>2</v>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+      <c r="H59" s="4" t="n">
+        <v>45713</v>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>Deepanshu Sharma</t>
+        </is>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>2</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>SB2/US27</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>add validation for embedding dimensions</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>consistency is ensured</t>
+        </is>
+      </c>
+      <c r="F60" t="n">
+        <v>2</v>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+      <c r="H60" s="4" t="n">
+        <v>45714</v>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>Deepanshu Sharma</t>
+        </is>
+      </c>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>2</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>SB2/US28</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>create embedding visualization tool</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>quality can be assessed</t>
+        </is>
+      </c>
+      <c r="F61" t="n">
+        <v>2</v>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+      <c r="H61" s="4" t="n">
+        <v>45715</v>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>Deepanshu Sharma</t>
+        </is>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>2</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>SB2/US29</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>implement incremental knowledge base updates</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>new content can be added</t>
+        </is>
+      </c>
+      <c r="F62" t="n">
+        <v>2</v>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+      <c r="H62" s="4" t="n">
+        <v>45716</v>
+      </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>Deepanshu Sharma</t>
+        </is>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>2</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>SB2/US30</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>create knowledge base documentation</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>structure is clear</t>
+        </is>
+      </c>
+      <c r="F63" t="n">
+        <v>1</v>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+      <c r="H63" s="4" t="n">
+        <v>45717</v>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>Deepanshu Sharma</t>
+        </is>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>3</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>SB3/US1</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>set up FastAPI framework</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>REST API can be built</t>
+        </is>
+      </c>
+      <c r="F64" t="n">
+        <v>1</v>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H64" s="4" t="n">
+        <v>45718</v>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>3</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>SB3/US2</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>configure CORS middleware</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>API is accessible from browsers</t>
+        </is>
+      </c>
+      <c r="F65" t="n">
+        <v>1</v>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H65" s="4" t="n">
+        <v>45719</v>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>3</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>SB3/US3</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>create Pydantic models</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>request/response data is validated</t>
+        </is>
+      </c>
+      <c r="F66" t="n">
+        <v>1</v>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H66" s="4" t="n">
+        <v>45720</v>
+      </c>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L66" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>3</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>SB3/US4</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>implement environment variable loading</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>configuration is secure</t>
+        </is>
+      </c>
+      <c r="F67" t="n">
+        <v>1</v>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H67" s="4" t="n">
+        <v>45721</v>
+      </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L67" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>3</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>SB3/US5</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>connect to SQLite database</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>knowledge base can be queried</t>
+        </is>
+      </c>
+      <c r="F68" t="n">
+        <v>1</v>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H68" s="4" t="n">
+        <v>45722</v>
+      </c>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L68" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>3</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>SB3/US6</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>load embedding model</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>queries can be embedded</t>
+        </is>
+      </c>
+      <c r="F69" t="n">
+        <v>1</v>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H69" s="4" t="n">
+        <v>45723</v>
+      </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L69" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>3</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>SB3/US7</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>implement query embedding</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>semantic search is possible</t>
+        </is>
+      </c>
+      <c r="F70" t="n">
+        <v>1</v>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H70" s="4" t="n">
+        <v>45724</v>
+      </c>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L70" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>3</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>SB3/US8</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>implement cosine similarity calculation</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>relevant chunks are found</t>
+        </is>
+      </c>
+      <c r="F71" t="n">
+        <v>1</v>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H71" s="4" t="n">
+        <v>45725</v>
+      </c>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L71" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>3</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>SB3/US9</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>implement database retrieval</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>relevant chunks are fetched</t>
+        </is>
+      </c>
+      <c r="F72" t="n">
+        <v>1</v>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H72" s="4" t="n">
+        <v>45726</v>
+      </c>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L72" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>3</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>SB3/US10</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>implement top-k filtering</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>only best results are returned</t>
+        </is>
+      </c>
+      <c r="F73" t="n">
+        <v>1</v>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H73" s="4" t="n">
+        <v>45727</v>
+      </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L73" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>3</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>SB3/US11</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>implement similarity threshold</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>low-quality results are excluded</t>
+        </is>
+      </c>
+      <c r="F74" t="n">
+        <v>1</v>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H74" s="4" t="n">
+        <v>45728</v>
+      </c>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L74" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>3</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>SB3/US12</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>integrate Tesseract OCR</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>images can be processed</t>
+        </is>
+      </c>
+      <c r="F75" t="n">
+        <v>2</v>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H75" s="4" t="n">
+        <v>45729</v>
+      </c>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L75" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>3</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>SB3/US13</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>implement base64 image decoding</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>images can be received</t>
+        </is>
+      </c>
+      <c r="F76" t="n">
+        <v>2</v>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H76" s="4" t="n">
+        <v>45730</v>
+      </c>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L76" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>3</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>SB3/US14</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>extract text from images</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>image queries are supported</t>
+        </is>
+      </c>
+      <c r="F77" t="n">
+        <v>2</v>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H77" s="4" t="n">
+        <v>45731</v>
+      </c>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L77" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>3</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>SB3/US15</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>handle OCR errors</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>API doesnt crash on bad images</t>
+        </is>
+      </c>
+      <c r="F78" t="n">
+        <v>2</v>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H78" s="4" t="n">
+        <v>45732</v>
+      </c>
+      <c r="K78" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L78" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>3</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>SB3/US16</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>integrate LLM API</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>answers can be generated</t>
+        </is>
+      </c>
+      <c r="F79" t="n">
+        <v>1</v>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>GM</t>
+        </is>
+      </c>
+      <c r="H79" s="4" t="n">
+        <v>45733</v>
+      </c>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>Gaurav Malik</t>
+        </is>
+      </c>
+      <c r="L79" t="inlineStr">
+        <is>
+          <t>GM</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>3</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>SB3/US17</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>create context prompt</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>LLM has relevant information</t>
+        </is>
+      </c>
+      <c r="F80" t="n">
+        <v>1</v>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>GM</t>
+        </is>
+      </c>
+      <c r="H80" s="4" t="n">
+        <v>45734</v>
+      </c>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>Gaurav Malik</t>
+        </is>
+      </c>
+      <c r="L80" t="inlineStr">
+        <is>
+          <t>GM</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>3</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>SB3/US18</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>implement answer generation</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>coherent responses are produced</t>
+        </is>
+      </c>
+      <c r="F81" t="n">
+        <v>1</v>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>GM</t>
+        </is>
+      </c>
+      <c r="H81" s="4" t="n">
+        <v>45735</v>
+      </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>Gaurav Malik</t>
+        </is>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>GM</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>3</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>SB3/US19</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>extract source URLs</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>citations are provided</t>
+        </is>
+      </c>
+      <c r="F82" t="n">
+        <v>1</v>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>GM</t>
+        </is>
+      </c>
+      <c r="H82" s="4" t="n">
+        <v>45736</v>
+      </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>Gaurav Malik</t>
+        </is>
+      </c>
+      <c r="L82" t="inlineStr">
+        <is>
+          <t>GM</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>3</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>SB3/US20</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>create structured response</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>API output is consistent</t>
+        </is>
+      </c>
+      <c r="F83" t="n">
+        <v>1</v>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>GM</t>
+        </is>
+      </c>
+      <c r="H83" s="4" t="n">
+        <v>45737</v>
+      </c>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>Gaurav Malik</t>
+        </is>
+      </c>
+      <c r="L83" t="inlineStr">
+        <is>
+          <t>GM</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>3</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>SB3/US21</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>implement /query endpoint</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>users can ask questions</t>
+        </is>
+      </c>
+      <c r="F84" t="n">
+        <v>1</v>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>GM</t>
+        </is>
+      </c>
+      <c r="H84" s="4" t="n">
+        <v>45738</v>
+      </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>Gaurav Malik</t>
+        </is>
+      </c>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t>GM</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>3</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>SB3/US22</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>implement request logging</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>usage can be tracked</t>
+        </is>
+      </c>
+      <c r="F85" t="n">
+        <v>2</v>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>GM</t>
+        </is>
+      </c>
+      <c r="H85" s="4" t="n">
+        <v>45739</v>
+      </c>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>Gaurav Malik</t>
+        </is>
+      </c>
+      <c r="L85" t="inlineStr">
+        <is>
+          <t>GM</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>3</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>SB3/US23</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>implement error handling</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>API is robust</t>
+        </is>
+      </c>
+      <c r="F86" t="n">
+        <v>1</v>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+      <c r="H86" s="4" t="n">
+        <v>45740</v>
+      </c>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>Deepanshu Sharma</t>
+        </is>
+      </c>
+      <c r="L86" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>3</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>SB3/US24</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>add API documentation</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>endpoints are well-described</t>
+        </is>
+      </c>
+      <c r="F87" t="n">
+        <v>2</v>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+      <c r="H87" s="4" t="n">
+        <v>45741</v>
+      </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>Deepanshu Sharma</t>
+        </is>
+      </c>
+      <c r="L87" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>3</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>SB3/US25</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>implement health check endpoint</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>API status can be monitored</t>
+        </is>
+      </c>
+      <c r="F88" t="n">
+        <v>2</v>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+      <c r="H88" s="4" t="n">
+        <v>45742</v>
+      </c>
+      <c r="K88" t="inlineStr">
+        <is>
+          <t>Deepanshu Sharma</t>
+        </is>
+      </c>
+      <c r="L88" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>3</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>SB3/US26</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>add request validation</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>invalid inputs are rejected</t>
+        </is>
+      </c>
+      <c r="F89" t="n">
+        <v>1</v>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+      <c r="H89" s="4" t="n">
+        <v>45743</v>
+      </c>
+      <c r="K89" t="inlineStr">
+        <is>
+          <t>Deepanshu Sharma</t>
+        </is>
+      </c>
+      <c r="L89" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>3</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>SB3/US27</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>implement rate limiting</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>API is not abused</t>
+        </is>
+      </c>
+      <c r="F90" t="n">
+        <v>2</v>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+      <c r="H90" s="4" t="n">
+        <v>45744</v>
+      </c>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>Deepanshu Sharma</t>
+        </is>
+      </c>
+      <c r="L90" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>3</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>SB3/US28</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>optimize response time</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>queries are fast</t>
+        </is>
+      </c>
+      <c r="F91" t="n">
+        <v>1</v>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+      <c r="H91" s="4" t="n">
+        <v>45745</v>
+      </c>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>Deepanshu Sharma</t>
+        </is>
+      </c>
+      <c r="L91" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>3</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>SB3/US29</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>add metrics collection</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>performance can be monitored</t>
+        </is>
+      </c>
+      <c r="F92" t="n">
+        <v>2</v>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+      <c r="H92" s="4" t="n">
+        <v>45746</v>
+      </c>
+      <c r="K92" t="inlineStr">
+        <is>
+          <t>Deepanshu Sharma</t>
+        </is>
+      </c>
+      <c r="L92" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>3</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>SB3/US30</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>create API testing suite</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>functionality is verified</t>
+        </is>
+      </c>
+      <c r="F93" t="n">
+        <v>1</v>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+      <c r="H93" s="4" t="n">
+        <v>45747</v>
+      </c>
+      <c r="K93" t="inlineStr">
+        <is>
+          <t>Deepanshu Sharma</t>
+        </is>
+      </c>
+      <c r="L93" t="inlineStr">
+        <is>
+          <t>DS</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update project dates to 2025-08-01 to 2025-11-20 and format dates without time
Co-authored-by: HarshChoudhary10 <144003686+HarshChoudhary10@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/PB.xlsx
+++ b/PB.xlsx
@@ -16,8 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -67,7 +68,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -79,6 +80,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -488,8 +490,6 @@
           <t>BACKLOG ITEM</t>
         </is>
       </c>
-      <c r="D2" s="2" t="n"/>
-      <c r="E2" s="2" t="n"/>
       <c r="F2" s="2" t="inlineStr">
         <is>
           <t>PRIORITY</t>
@@ -582,8 +582,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H4" s="4" t="n">
-        <v>45672</v>
+      <c r="H4" s="5" t="n">
+        <v>45870</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
@@ -628,8 +628,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H5" s="4" t="n">
-        <v>45672</v>
+      <c r="H5" s="5" t="n">
+        <v>45871</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
@@ -674,8 +674,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H6" s="4" t="n">
-        <v>45673</v>
+      <c r="H6" s="5" t="n">
+        <v>45872</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
@@ -720,8 +720,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H7" s="4" t="n">
-        <v>45673</v>
+      <c r="H7" s="5" t="n">
+        <v>45873</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
@@ -766,8 +766,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H8" s="4" t="n">
-        <v>45673</v>
+      <c r="H8" s="5" t="n">
+        <v>45874</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
@@ -812,8 +812,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H9" s="4" t="n">
-        <v>45674</v>
+      <c r="H9" s="5" t="n">
+        <v>45875</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
@@ -858,8 +858,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H10" s="4" t="n">
-        <v>45675</v>
+      <c r="H10" s="5" t="n">
+        <v>45876</v>
       </c>
       <c r="K10" t="inlineStr">
         <is>
@@ -904,8 +904,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H11" s="4" t="n">
-        <v>45676</v>
+      <c r="H11" s="5" t="n">
+        <v>45877</v>
       </c>
       <c r="K11" t="inlineStr">
         <is>
@@ -950,8 +950,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H12" s="4" t="n">
-        <v>45676</v>
+      <c r="H12" s="5" t="n">
+        <v>45878</v>
       </c>
       <c r="K12" t="inlineStr">
         <is>
@@ -996,8 +996,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H13" s="4" t="n">
-        <v>45677</v>
+      <c r="H13" s="5" t="n">
+        <v>45879</v>
       </c>
       <c r="K13" t="inlineStr">
         <is>
@@ -1042,8 +1042,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H14" s="4" t="n">
-        <v>45677</v>
+      <c r="H14" s="5" t="n">
+        <v>45880</v>
       </c>
       <c r="K14" t="inlineStr">
         <is>
@@ -1088,8 +1088,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H15" s="4" t="n">
-        <v>45677</v>
+      <c r="H15" s="5" t="n">
+        <v>45881</v>
       </c>
       <c r="K15" t="inlineStr">
         <is>
@@ -1134,8 +1134,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H16" s="4" t="n">
-        <v>45678</v>
+      <c r="H16" s="5" t="n">
+        <v>45882</v>
       </c>
       <c r="K16" t="inlineStr">
         <is>
@@ -1180,8 +1180,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H17" s="4" t="n">
-        <v>45678</v>
+      <c r="H17" s="5" t="n">
+        <v>45883</v>
       </c>
       <c r="K17" t="inlineStr">
         <is>
@@ -1226,8 +1226,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H18" s="4" t="n">
-        <v>45679</v>
+      <c r="H18" s="5" t="n">
+        <v>45884</v>
       </c>
       <c r="K18" t="inlineStr">
         <is>
@@ -1272,8 +1272,8 @@
           <t>GM</t>
         </is>
       </c>
-      <c r="H19" s="4" t="n">
-        <v>45679</v>
+      <c r="H19" s="5" t="n">
+        <v>45885</v>
       </c>
       <c r="K19" t="inlineStr">
         <is>
@@ -1318,8 +1318,8 @@
           <t>GM</t>
         </is>
       </c>
-      <c r="H20" s="4" t="n">
-        <v>45680</v>
+      <c r="H20" s="5" t="n">
+        <v>45886</v>
       </c>
       <c r="K20" t="inlineStr">
         <is>
@@ -1364,8 +1364,8 @@
           <t>GM</t>
         </is>
       </c>
-      <c r="H21" s="4" t="n">
-        <v>45680</v>
+      <c r="H21" s="5" t="n">
+        <v>45887</v>
       </c>
       <c r="K21" t="inlineStr">
         <is>
@@ -1410,8 +1410,8 @@
           <t>GM</t>
         </is>
       </c>
-      <c r="H22" s="4" t="n">
-        <v>45681</v>
+      <c r="H22" s="5" t="n">
+        <v>45888</v>
       </c>
       <c r="K22" t="inlineStr">
         <is>
@@ -1456,8 +1456,8 @@
           <t>GM</t>
         </is>
       </c>
-      <c r="H23" s="4" t="n">
-        <v>45681</v>
+      <c r="H23" s="5" t="n">
+        <v>45889</v>
       </c>
       <c r="K23" t="inlineStr">
         <is>
@@ -1502,8 +1502,8 @@
           <t>GM</t>
         </is>
       </c>
-      <c r="H24" s="4" t="n">
-        <v>45682</v>
+      <c r="H24" s="5" t="n">
+        <v>45890</v>
       </c>
       <c r="K24" t="inlineStr">
         <is>
@@ -1548,8 +1548,8 @@
           <t>GM</t>
         </is>
       </c>
-      <c r="H25" s="4" t="n">
-        <v>45682</v>
+      <c r="H25" s="5" t="n">
+        <v>45891</v>
       </c>
       <c r="K25" t="inlineStr">
         <is>
@@ -1594,8 +1594,8 @@
           <t>DS</t>
         </is>
       </c>
-      <c r="H26" s="4" t="n">
-        <v>45683</v>
+      <c r="H26" s="5" t="n">
+        <v>45892</v>
       </c>
       <c r="K26" t="inlineStr">
         <is>
@@ -1640,8 +1640,8 @@
           <t>DS</t>
         </is>
       </c>
-      <c r="H27" s="4" t="n">
-        <v>45683</v>
+      <c r="H27" s="5" t="n">
+        <v>45893</v>
       </c>
       <c r="K27" t="inlineStr">
         <is>
@@ -1686,8 +1686,8 @@
           <t>DS</t>
         </is>
       </c>
-      <c r="H28" s="4" t="n">
-        <v>45684</v>
+      <c r="H28" s="5" t="n">
+        <v>45894</v>
       </c>
       <c r="K28" t="inlineStr">
         <is>
@@ -1732,8 +1732,8 @@
           <t>DS</t>
         </is>
       </c>
-      <c r="H29" s="4" t="n">
-        <v>45684</v>
+      <c r="H29" s="5" t="n">
+        <v>45895</v>
       </c>
       <c r="K29" t="inlineStr">
         <is>
@@ -1778,8 +1778,8 @@
           <t>DS</t>
         </is>
       </c>
-      <c r="H30" s="4" t="n">
-        <v>45685</v>
+      <c r="H30" s="5" t="n">
+        <v>45896</v>
       </c>
       <c r="K30" t="inlineStr">
         <is>
@@ -1824,8 +1824,8 @@
           <t>DS</t>
         </is>
       </c>
-      <c r="H31" s="4" t="n">
-        <v>45685</v>
+      <c r="H31" s="5" t="n">
+        <v>45897</v>
       </c>
       <c r="K31" t="inlineStr">
         <is>
@@ -1870,8 +1870,8 @@
           <t>DS</t>
         </is>
       </c>
-      <c r="H32" s="4" t="n">
-        <v>45686</v>
+      <c r="H32" s="5" t="n">
+        <v>45898</v>
       </c>
       <c r="K32" t="inlineStr">
         <is>
@@ -1916,8 +1916,8 @@
           <t>DS</t>
         </is>
       </c>
-      <c r="H33" s="4" t="n">
-        <v>45687</v>
+      <c r="H33" s="5" t="n">
+        <v>45899</v>
       </c>
       <c r="K33" t="inlineStr">
         <is>
@@ -1962,8 +1962,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H34" s="4" t="n">
-        <v>45688</v>
+      <c r="H34" s="5" t="n">
+        <v>45908</v>
       </c>
       <c r="K34" t="inlineStr">
         <is>
@@ -2008,8 +2008,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H35" s="4" t="n">
-        <v>45689</v>
+      <c r="H35" s="5" t="n">
+        <v>45909</v>
       </c>
       <c r="K35" t="inlineStr">
         <is>
@@ -2054,8 +2054,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H36" s="4" t="n">
-        <v>45690</v>
+      <c r="H36" s="5" t="n">
+        <v>45910</v>
       </c>
       <c r="K36" t="inlineStr">
         <is>
@@ -2100,8 +2100,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H37" s="4" t="n">
-        <v>45691</v>
+      <c r="H37" s="5" t="n">
+        <v>45911</v>
       </c>
       <c r="K37" t="inlineStr">
         <is>
@@ -2146,8 +2146,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H38" s="4" t="n">
-        <v>45692</v>
+      <c r="H38" s="5" t="n">
+        <v>45912</v>
       </c>
       <c r="K38" t="inlineStr">
         <is>
@@ -2192,8 +2192,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H39" s="4" t="n">
-        <v>45693</v>
+      <c r="H39" s="5" t="n">
+        <v>45913</v>
       </c>
       <c r="K39" t="inlineStr">
         <is>
@@ -2238,8 +2238,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H40" s="4" t="n">
-        <v>45694</v>
+      <c r="H40" s="5" t="n">
+        <v>45914</v>
       </c>
       <c r="K40" t="inlineStr">
         <is>
@@ -2284,8 +2284,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H41" s="4" t="n">
-        <v>45695</v>
+      <c r="H41" s="5" t="n">
+        <v>45915</v>
       </c>
       <c r="K41" t="inlineStr">
         <is>
@@ -2330,8 +2330,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H42" s="4" t="n">
-        <v>45696</v>
+      <c r="H42" s="5" t="n">
+        <v>45916</v>
       </c>
       <c r="K42" t="inlineStr">
         <is>
@@ -2376,8 +2376,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H43" s="4" t="n">
-        <v>45697</v>
+      <c r="H43" s="5" t="n">
+        <v>45917</v>
       </c>
       <c r="K43" t="inlineStr">
         <is>
@@ -2422,8 +2422,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H44" s="4" t="n">
-        <v>45698</v>
+      <c r="H44" s="5" t="n">
+        <v>45918</v>
       </c>
       <c r="K44" t="inlineStr">
         <is>
@@ -2468,8 +2468,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H45" s="4" t="n">
-        <v>45699</v>
+      <c r="H45" s="5" t="n">
+        <v>45919</v>
       </c>
       <c r="K45" t="inlineStr">
         <is>
@@ -2514,8 +2514,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H46" s="4" t="n">
-        <v>45700</v>
+      <c r="H46" s="5" t="n">
+        <v>45920</v>
       </c>
       <c r="K46" t="inlineStr">
         <is>
@@ -2560,8 +2560,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H47" s="4" t="n">
-        <v>45701</v>
+      <c r="H47" s="5" t="n">
+        <v>45921</v>
       </c>
       <c r="K47" t="inlineStr">
         <is>
@@ -2606,8 +2606,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H48" s="4" t="n">
-        <v>45702</v>
+      <c r="H48" s="5" t="n">
+        <v>45922</v>
       </c>
       <c r="K48" t="inlineStr">
         <is>
@@ -2652,8 +2652,8 @@
           <t>GM</t>
         </is>
       </c>
-      <c r="H49" s="4" t="n">
-        <v>45703</v>
+      <c r="H49" s="5" t="n">
+        <v>45923</v>
       </c>
       <c r="K49" t="inlineStr">
         <is>
@@ -2698,8 +2698,8 @@
           <t>GM</t>
         </is>
       </c>
-      <c r="H50" s="4" t="n">
-        <v>45704</v>
+      <c r="H50" s="5" t="n">
+        <v>45924</v>
       </c>
       <c r="K50" t="inlineStr">
         <is>
@@ -2744,8 +2744,8 @@
           <t>GM</t>
         </is>
       </c>
-      <c r="H51" s="4" t="n">
-        <v>45705</v>
+      <c r="H51" s="5" t="n">
+        <v>45925</v>
       </c>
       <c r="K51" t="inlineStr">
         <is>
@@ -2790,8 +2790,8 @@
           <t>GM</t>
         </is>
       </c>
-      <c r="H52" s="4" t="n">
-        <v>45706</v>
+      <c r="H52" s="5" t="n">
+        <v>45926</v>
       </c>
       <c r="K52" t="inlineStr">
         <is>
@@ -2836,8 +2836,8 @@
           <t>GM</t>
         </is>
       </c>
-      <c r="H53" s="4" t="n">
-        <v>45707</v>
+      <c r="H53" s="5" t="n">
+        <v>45927</v>
       </c>
       <c r="K53" t="inlineStr">
         <is>
@@ -2882,8 +2882,8 @@
           <t>GM</t>
         </is>
       </c>
-      <c r="H54" s="4" t="n">
-        <v>45708</v>
+      <c r="H54" s="5" t="n">
+        <v>45928</v>
       </c>
       <c r="K54" t="inlineStr">
         <is>
@@ -2928,8 +2928,8 @@
           <t>GM</t>
         </is>
       </c>
-      <c r="H55" s="4" t="n">
-        <v>45709</v>
+      <c r="H55" s="5" t="n">
+        <v>45929</v>
       </c>
       <c r="K55" t="inlineStr">
         <is>
@@ -2974,8 +2974,8 @@
           <t>DS</t>
         </is>
       </c>
-      <c r="H56" s="4" t="n">
-        <v>45710</v>
+      <c r="H56" s="5" t="n">
+        <v>45930</v>
       </c>
       <c r="K56" t="inlineStr">
         <is>
@@ -3020,8 +3020,8 @@
           <t>DS</t>
         </is>
       </c>
-      <c r="H57" s="4" t="n">
-        <v>45711</v>
+      <c r="H57" s="5" t="n">
+        <v>45931</v>
       </c>
       <c r="K57" t="inlineStr">
         <is>
@@ -3066,8 +3066,8 @@
           <t>DS</t>
         </is>
       </c>
-      <c r="H58" s="4" t="n">
-        <v>45712</v>
+      <c r="H58" s="5" t="n">
+        <v>45932</v>
       </c>
       <c r="K58" t="inlineStr">
         <is>
@@ -3112,8 +3112,8 @@
           <t>DS</t>
         </is>
       </c>
-      <c r="H59" s="4" t="n">
-        <v>45713</v>
+      <c r="H59" s="5" t="n">
+        <v>45933</v>
       </c>
       <c r="K59" t="inlineStr">
         <is>
@@ -3158,8 +3158,8 @@
           <t>DS</t>
         </is>
       </c>
-      <c r="H60" s="4" t="n">
-        <v>45714</v>
+      <c r="H60" s="5" t="n">
+        <v>45934</v>
       </c>
       <c r="K60" t="inlineStr">
         <is>
@@ -3204,8 +3204,8 @@
           <t>DS</t>
         </is>
       </c>
-      <c r="H61" s="4" t="n">
-        <v>45715</v>
+      <c r="H61" s="5" t="n">
+        <v>45935</v>
       </c>
       <c r="K61" t="inlineStr">
         <is>
@@ -3250,8 +3250,8 @@
           <t>DS</t>
         </is>
       </c>
-      <c r="H62" s="4" t="n">
-        <v>45716</v>
+      <c r="H62" s="5" t="n">
+        <v>45936</v>
       </c>
       <c r="K62" t="inlineStr">
         <is>
@@ -3296,8 +3296,8 @@
           <t>DS</t>
         </is>
       </c>
-      <c r="H63" s="4" t="n">
-        <v>45717</v>
+      <c r="H63" s="5" t="n">
+        <v>45937</v>
       </c>
       <c r="K63" t="inlineStr">
         <is>
@@ -3342,8 +3342,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H64" s="4" t="n">
-        <v>45718</v>
+      <c r="H64" s="5" t="n">
+        <v>45946</v>
       </c>
       <c r="K64" t="inlineStr">
         <is>
@@ -3388,8 +3388,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H65" s="4" t="n">
-        <v>45719</v>
+      <c r="H65" s="5" t="n">
+        <v>45947</v>
       </c>
       <c r="K65" t="inlineStr">
         <is>
@@ -3434,8 +3434,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H66" s="4" t="n">
-        <v>45720</v>
+      <c r="H66" s="5" t="n">
+        <v>45948</v>
       </c>
       <c r="K66" t="inlineStr">
         <is>
@@ -3480,8 +3480,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H67" s="4" t="n">
-        <v>45721</v>
+      <c r="H67" s="5" t="n">
+        <v>45949</v>
       </c>
       <c r="K67" t="inlineStr">
         <is>
@@ -3526,8 +3526,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H68" s="4" t="n">
-        <v>45722</v>
+      <c r="H68" s="5" t="n">
+        <v>45950</v>
       </c>
       <c r="K68" t="inlineStr">
         <is>
@@ -3572,8 +3572,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H69" s="4" t="n">
-        <v>45723</v>
+      <c r="H69" s="5" t="n">
+        <v>45951</v>
       </c>
       <c r="K69" t="inlineStr">
         <is>
@@ -3618,8 +3618,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H70" s="4" t="n">
-        <v>45724</v>
+      <c r="H70" s="5" t="n">
+        <v>45952</v>
       </c>
       <c r="K70" t="inlineStr">
         <is>
@@ -3664,8 +3664,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H71" s="4" t="n">
-        <v>45725</v>
+      <c r="H71" s="5" t="n">
+        <v>45953</v>
       </c>
       <c r="K71" t="inlineStr">
         <is>
@@ -3710,8 +3710,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H72" s="4" t="n">
-        <v>45726</v>
+      <c r="H72" s="5" t="n">
+        <v>45954</v>
       </c>
       <c r="K72" t="inlineStr">
         <is>
@@ -3756,8 +3756,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H73" s="4" t="n">
-        <v>45727</v>
+      <c r="H73" s="5" t="n">
+        <v>45955</v>
       </c>
       <c r="K73" t="inlineStr">
         <is>
@@ -3802,8 +3802,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H74" s="4" t="n">
-        <v>45728</v>
+      <c r="H74" s="5" t="n">
+        <v>45956</v>
       </c>
       <c r="K74" t="inlineStr">
         <is>
@@ -3848,8 +3848,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H75" s="4" t="n">
-        <v>45729</v>
+      <c r="H75" s="5" t="n">
+        <v>45957</v>
       </c>
       <c r="K75" t="inlineStr">
         <is>
@@ -3894,8 +3894,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H76" s="4" t="n">
-        <v>45730</v>
+      <c r="H76" s="5" t="n">
+        <v>45958</v>
       </c>
       <c r="K76" t="inlineStr">
         <is>
@@ -3940,8 +3940,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H77" s="4" t="n">
-        <v>45731</v>
+      <c r="H77" s="5" t="n">
+        <v>45959</v>
       </c>
       <c r="K77" t="inlineStr">
         <is>
@@ -3986,8 +3986,8 @@
           <t>HC</t>
         </is>
       </c>
-      <c r="H78" s="4" t="n">
-        <v>45732</v>
+      <c r="H78" s="5" t="n">
+        <v>45960</v>
       </c>
       <c r="K78" t="inlineStr">
         <is>
@@ -4032,8 +4032,8 @@
           <t>GM</t>
         </is>
       </c>
-      <c r="H79" s="4" t="n">
-        <v>45733</v>
+      <c r="H79" s="5" t="n">
+        <v>45961</v>
       </c>
       <c r="K79" t="inlineStr">
         <is>
@@ -4078,8 +4078,8 @@
           <t>GM</t>
         </is>
       </c>
-      <c r="H80" s="4" t="n">
-        <v>45734</v>
+      <c r="H80" s="5" t="n">
+        <v>45962</v>
       </c>
       <c r="K80" t="inlineStr">
         <is>
@@ -4124,8 +4124,8 @@
           <t>GM</t>
         </is>
       </c>
-      <c r="H81" s="4" t="n">
-        <v>45735</v>
+      <c r="H81" s="5" t="n">
+        <v>45963</v>
       </c>
       <c r="K81" t="inlineStr">
         <is>
@@ -4170,8 +4170,8 @@
           <t>GM</t>
         </is>
       </c>
-      <c r="H82" s="4" t="n">
-        <v>45736</v>
+      <c r="H82" s="5" t="n">
+        <v>45964</v>
       </c>
       <c r="K82" t="inlineStr">
         <is>
@@ -4216,8 +4216,8 @@
           <t>GM</t>
         </is>
       </c>
-      <c r="H83" s="4" t="n">
-        <v>45737</v>
+      <c r="H83" s="5" t="n">
+        <v>45965</v>
       </c>
       <c r="K83" t="inlineStr">
         <is>
@@ -4262,8 +4262,8 @@
           <t>GM</t>
         </is>
       </c>
-      <c r="H84" s="4" t="n">
-        <v>45738</v>
+      <c r="H84" s="5" t="n">
+        <v>45966</v>
       </c>
       <c r="K84" t="inlineStr">
         <is>
@@ -4308,8 +4308,8 @@
           <t>GM</t>
         </is>
       </c>
-      <c r="H85" s="4" t="n">
-        <v>45739</v>
+      <c r="H85" s="5" t="n">
+        <v>45967</v>
       </c>
       <c r="K85" t="inlineStr">
         <is>
@@ -4354,8 +4354,8 @@
           <t>DS</t>
         </is>
       </c>
-      <c r="H86" s="4" t="n">
-        <v>45740</v>
+      <c r="H86" s="5" t="n">
+        <v>45968</v>
       </c>
       <c r="K86" t="inlineStr">
         <is>
@@ -4400,8 +4400,8 @@
           <t>DS</t>
         </is>
       </c>
-      <c r="H87" s="4" t="n">
-        <v>45741</v>
+      <c r="H87" s="5" t="n">
+        <v>45969</v>
       </c>
       <c r="K87" t="inlineStr">
         <is>
@@ -4446,8 +4446,8 @@
           <t>DS</t>
         </is>
       </c>
-      <c r="H88" s="4" t="n">
-        <v>45742</v>
+      <c r="H88" s="5" t="n">
+        <v>45970</v>
       </c>
       <c r="K88" t="inlineStr">
         <is>
@@ -4492,8 +4492,8 @@
           <t>DS</t>
         </is>
       </c>
-      <c r="H89" s="4" t="n">
-        <v>45743</v>
+      <c r="H89" s="5" t="n">
+        <v>45971</v>
       </c>
       <c r="K89" t="inlineStr">
         <is>
@@ -4538,8 +4538,8 @@
           <t>DS</t>
         </is>
       </c>
-      <c r="H90" s="4" t="n">
-        <v>45744</v>
+      <c r="H90" s="5" t="n">
+        <v>45972</v>
       </c>
       <c r="K90" t="inlineStr">
         <is>
@@ -4584,8 +4584,8 @@
           <t>DS</t>
         </is>
       </c>
-      <c r="H91" s="4" t="n">
-        <v>45745</v>
+      <c r="H91" s="5" t="n">
+        <v>45973</v>
       </c>
       <c r="K91" t="inlineStr">
         <is>
@@ -4630,8 +4630,8 @@
           <t>DS</t>
         </is>
       </c>
-      <c r="H92" s="4" t="n">
-        <v>45746</v>
+      <c r="H92" s="5" t="n">
+        <v>45974</v>
       </c>
       <c r="K92" t="inlineStr">
         <is>
@@ -4676,8 +4676,8 @@
           <t>DS</t>
         </is>
       </c>
-      <c r="H93" s="4" t="n">
-        <v>45747</v>
+      <c r="H93" s="5" t="n">
+        <v>45975</v>
       </c>
       <c r="K93" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Add Sprint Backlog 4 and update Product Backlog for frontend development
Co-authored-by: HarshChoudhary10 <144003686+HarshChoudhary10@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/PB.xlsx
+++ b/PB.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M93"/>
+  <dimension ref="A1:M123"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4690,6 +4690,1386 @@
         </is>
       </c>
     </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>4</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>SB4/US1</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>design the frontend architecture</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>the UI is well-structured</t>
+        </is>
+      </c>
+      <c r="F94" t="n">
+        <v>4</v>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H94" s="4" t="n">
+        <v>45992</v>
+      </c>
+      <c r="K94" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L94" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>4</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>SB4/US2</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>create the HTML structure</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>the UI has proper semantic markup</t>
+        </is>
+      </c>
+      <c r="F95" t="n">
+        <v>4</v>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H95" s="4" t="n">
+        <v>45995</v>
+      </c>
+      <c r="K95" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L95" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>4</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>SB4/US3</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>implement CSS styling</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>the interface is visually appealing</t>
+        </is>
+      </c>
+      <c r="F96" t="n">
+        <v>4</v>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H96" s="4" t="n">
+        <v>45998</v>
+      </c>
+      <c r="K96" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L96" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>4</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>SB4/US4</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>implement JavaScript functionality</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>the frontend interacts with the API</t>
+        </is>
+      </c>
+      <c r="F97" t="n">
+        <v>4</v>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H97" s="4" t="n">
+        <v>46001</v>
+      </c>
+      <c r="K97" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L97" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>4</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>SB4/US5</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>User</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>submit questions</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>I can get answers from the Virtual TA</t>
+        </is>
+      </c>
+      <c r="F98" t="n">
+        <v>4</v>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H98" s="4" t="n">
+        <v>46004</v>
+      </c>
+      <c r="K98" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L98" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>4</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>SB4/US6</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>User</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>upload images</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>the TA can analyze screenshots</t>
+        </is>
+      </c>
+      <c r="F99" t="n">
+        <v>4</v>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H99" s="4" t="n">
+        <v>46007</v>
+      </c>
+      <c r="K99" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L99" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>4</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>SB4/US7</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>User</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>view answers</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>I can get information from the Virtual TA</t>
+        </is>
+      </c>
+      <c r="F100" t="n">
+        <v>4</v>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H100" s="4" t="n">
+        <v>46010</v>
+      </c>
+      <c r="K100" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L100" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>4</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>SB4/US8</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>implement error handling</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>users get helpful feedback</t>
+        </is>
+      </c>
+      <c r="F101" t="n">
+        <v>4</v>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H101" s="4" t="n">
+        <v>46013</v>
+      </c>
+      <c r="K101" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L101" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>4</v>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>SB4/US9</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>add CORS support</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>the API works with the frontend</t>
+        </is>
+      </c>
+      <c r="F102" t="n">
+        <v>4</v>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H102" s="4" t="n">
+        <v>46016</v>
+      </c>
+      <c r="K102" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L102" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>4</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>SB4/US10</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>create a chat history feature</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>users can review past queries</t>
+        </is>
+      </c>
+      <c r="F103" t="n">
+        <v>4</v>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H103" s="4" t="n">
+        <v>46019</v>
+      </c>
+      <c r="K103" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L103" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>4</v>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>SB4/US11</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>User</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>the interface to be responsive</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>I can use it on mobile devices</t>
+        </is>
+      </c>
+      <c r="F104" t="n">
+        <v>4</v>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H104" s="4" t="n">
+        <v>46022</v>
+      </c>
+      <c r="K104" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L104" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>4</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>SB4/US12</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>optimize performance</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>the app loads quickly</t>
+        </is>
+      </c>
+      <c r="F105" t="n">
+        <v>4</v>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H105" s="4" t="n">
+        <v>46025</v>
+      </c>
+      <c r="K105" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L105" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>4</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>SB4/US13</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>add accessibility features</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>the app is usable by everyone</t>
+        </is>
+      </c>
+      <c r="F106" t="n">
+        <v>4</v>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H106" s="4" t="n">
+        <v>46028</v>
+      </c>
+      <c r="K106" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L106" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>4</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>SB4/US14</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>create frontend documentation</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>others can understand the code</t>
+        </is>
+      </c>
+      <c r="F107" t="n">
+        <v>4</v>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H107" s="4" t="n">
+        <v>46031</v>
+      </c>
+      <c r="K107" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L107" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>4</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>SB4/US15</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>test the frontend</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>bugs are caught early</t>
+        </is>
+      </c>
+      <c r="F108" t="n">
+        <v>4</v>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H108" s="4" t="n">
+        <v>46034</v>
+      </c>
+      <c r="K108" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L108" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>4</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>SB4/US16</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>deploy the frontend</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>users can access it</t>
+        </is>
+      </c>
+      <c r="F109" t="n">
+        <v>4</v>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H109" s="4" t="n">
+        <v>46037</v>
+      </c>
+      <c r="K109" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L109" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>4</v>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>SB4/US17</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>add theme support</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>users can customize appearance</t>
+        </is>
+      </c>
+      <c r="F110" t="n">
+        <v>4</v>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H110" s="4" t="n">
+        <v>46040</v>
+      </c>
+      <c r="K110" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L110" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>4</v>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>SB4/US18</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>integrate API endpoint</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>frontend can communicate with backend</t>
+        </is>
+      </c>
+      <c r="F111" t="n">
+        <v>4</v>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H111" s="4" t="n">
+        <v>46043</v>
+      </c>
+      <c r="K111" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L111" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>4</v>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>SB4/US19</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>User</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>see example queries</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>I know what to ask</t>
+        </is>
+      </c>
+      <c r="F112" t="n">
+        <v>4</v>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H112" s="4" t="n">
+        <v>46046</v>
+      </c>
+      <c r="K112" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L112" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>4</v>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>SB4/US20</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>add analytics tracking</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>usage can be monitored</t>
+        </is>
+      </c>
+      <c r="F113" t="n">
+        <v>4</v>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H113" s="4" t="n">
+        <v>46049</v>
+      </c>
+      <c r="K113" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L113" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>4</v>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>SB4/US21</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>create a landing page</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>users understand the Virtual TA</t>
+        </is>
+      </c>
+      <c r="F114" t="n">
+        <v>4</v>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H114" s="4" t="n">
+        <v>46052</v>
+      </c>
+      <c r="K114" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L114" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>4</v>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>SB4/US22</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>add loading animations</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>users know the app is working</t>
+        </is>
+      </c>
+      <c r="F115" t="n">
+        <v>4</v>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H115" s="4" t="n">
+        <v>46055</v>
+      </c>
+      <c r="K115" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L115" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>4</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>SB4/US23</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>User</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>copy answers</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>I can save useful information</t>
+        </is>
+      </c>
+      <c r="F116" t="n">
+        <v>4</v>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H116" s="4" t="n">
+        <v>46058</v>
+      </c>
+      <c r="K116" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L116" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>4</v>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>SB4/US24</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>implement rate limiting</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>API is not overwhelmed</t>
+        </is>
+      </c>
+      <c r="F117" t="n">
+        <v>4</v>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H117" s="4" t="n">
+        <v>46061</v>
+      </c>
+      <c r="K117" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L117" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>4</v>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>SB4/US25</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>add final polish</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>the frontend is production-ready</t>
+        </is>
+      </c>
+      <c r="F118" t="n">
+        <v>4</v>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H118" s="4" t="n">
+        <v>46064</v>
+      </c>
+      <c r="K118" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L118" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>4</v>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>SB4/US26</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>update project documentation</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>Sprint 4 work is captured</t>
+        </is>
+      </c>
+      <c r="F119" t="n">
+        <v>4</v>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H119" s="4" t="n">
+        <v>46067</v>
+      </c>
+      <c r="K119" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L119" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>4</v>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>SB4/US27</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>create user guide</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>users know how to use the Virtual TA</t>
+        </is>
+      </c>
+      <c r="F120" t="n">
+        <v>4</v>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H120" s="4" t="n">
+        <v>46070</v>
+      </c>
+      <c r="K120" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L120" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>4</v>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>SB4/US28</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>implement feedback mechanism</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>users can report issues</t>
+        </is>
+      </c>
+      <c r="F121" t="n">
+        <v>4</v>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H121" s="4" t="n">
+        <v>46073</v>
+      </c>
+      <c r="K121" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L121" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>4</v>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>SB4/US29</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>configure CI/CD</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>frontend deploys automatically</t>
+        </is>
+      </c>
+      <c r="F122" t="n">
+        <v>4</v>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H122" s="4" t="n">
+        <v>46076</v>
+      </c>
+      <c r="K122" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L122" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>4</v>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>SB4/US30</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>conduct final review</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>Sprint 4 is complete</t>
+        </is>
+      </c>
+      <c r="F123" t="n">
+        <v>4</v>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="H123" s="4" t="n">
+        <v>46079</v>
+      </c>
+      <c r="K123" t="inlineStr">
+        <is>
+          <t>Harsh Choudhary</t>
+        </is>
+      </c>
+      <c r="L123" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C2:E2"/>

</xml_diff>